<commit_message>
remove not sure results
</commit_message>
<xml_diff>
--- a/xlsx/dumped_-1.xlsx
+++ b/xlsx/dumped_-1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,109 +470,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Evolution of Type-1 Clones</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>N. G√∂de</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2009</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>10.1109/SCAM.2009.17</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>978-0-7695-3793-1</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>https://ieeexplore.ieee.org/stamp/stamp.jsp?arnumber=5279977</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Clone detection: Why, what and how?</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>M. Akhin; V. Itsykson</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2010</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>10.1109/CEE-SECR.2010.5783148</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>978-1-4577-0606-6</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>https://ieeexplore.ieee.org/stamp/stamp.jsp?arnumber=5783148</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>LibDX: A Cross-Platform and Accurate System to Detect Third-Party Libraries in Binary Code</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>W. Tang; P. Luo; J. Fu; D. Zhang</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>10.1109/SANER48275.2020.9054845</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>978-1-7281-5143-4</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>1534-5351</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>https://ieeexplore.ieee.org/stamp/stamp.jsp?arnumber=9054845</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>